<commit_message>
modified notebook for temporal clustering, added plots of patterns'
</commit_message>
<xml_diff>
--- a/temporal_clustering/data/outputs/adf_table_before_difference.xlsx
+++ b/temporal_clustering/data/outputs/adf_table_before_difference.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\常用\NYU\IAQF\IAQF22\temporal_clustering\data\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1028066E-A8D1-4EF7-9DC4-A567568E0B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2025326F-DCEB-4587-95BF-6EECA518E953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="58815" yWindow="2955" windowWidth="16455" windowHeight="9555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="adf_table_before_difference" sheetId="1" r:id="rId1"/>
@@ -71,14 +71,14 @@
   </si>
   <si>
     <t>Reject at 5%?</t>
-    <phoneticPr fontId="19" type="noConversion"/>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,21 +232,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <i/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -433,7 +440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -549,55 +556,99 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="dotted">
+        <color theme="1"/>
+      </top>
+      <bottom style="dotted">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="dotted">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color theme="1"/>
+      </top>
+      <bottom style="dotted">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -730,36 +781,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1115,201 +1187,237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.0703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.0703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.0703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>3.3576999999999999</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>-6.6337000000000002</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>0</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>5.2309000000000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>1</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>-2.4417</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>0.1303</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>-2.2172000000000001</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>0.2001</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>-0.95779999999999998</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>0.76839999999999997</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>0.30620000000000003</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>0.97760000000000002</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <v>-1.2807999999999999</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>0.63790000000000002</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <v>-0.72670000000000001</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>0.8397</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="7">
         <v>-2.2845</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>0.17699999999999999</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="7">
         <v>-1.7667999999999999</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <v>0.39710000000000001</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:9" s="8" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="9">
@@ -1318,13 +1426,28 @@
       <c r="C14" s="9">
         <v>7.1800000000000003E-2</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>